<commit_message>
se descargo el syllabus
</commit_message>
<xml_diff>
--- a/HORARIO LOAYZA.xlsx
+++ b/HORARIO LOAYZA.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aguirre\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kleberAndres\Documents\universidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -705,8 +705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
se termino la clase de informatica aplicada
</commit_message>
<xml_diff>
--- a/HORARIO LOAYZA.xlsx
+++ b/HORARIO LOAYZA.xlsx
@@ -261,7 +261,7 @@
     <t>CAPACITACIÓN CONTINUA ECONOMÍA</t>
   </si>
   <si>
-    <t>Practicas PreProf</t>
+    <t>Practicas PreProf Economia</t>
   </si>
 </sst>
 </file>
@@ -703,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,7 +714,7 @@
     <col min="3" max="3" width="14.5703125" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -946,7 +946,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>25</v>
       </c>

</xml_diff>